<commit_message>
Adjust 'Count' parameter in NBHF detections
The number of clicks 'Count' was not being saved properly in the detection metadata. I adjusted the source map as well as the code to generate the detection worksheets for NBHF data.
</commit_message>
<xml_diff>
--- a/Detection Worksheets/CCES010_NBHF_Detections.xlsx
+++ b/Detection Worksheets/CCES010_NBHF_Detections.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="33">
   <si>
     <t xml:space="preserve">User ID</t>
   </si>
@@ -74,22 +74,7 @@
     <t xml:space="preserve">Granularity</t>
   </si>
   <si>
-    <t xml:space="preserve">Parameter 1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X..1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X..2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X..3</t>
-  </si>
-  <si>
-    <t xml:space="preserve">X..4</t>
+    <t xml:space="preserve">Count</t>
   </si>
   <si>
     <t xml:space="preserve">Other Odontocetes</t>
@@ -102,9 +87,6 @@
   </si>
   <si>
     <t xml:space="preserve">encounter</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nClicks</t>
   </si>
   <si>
     <t xml:space="preserve"/>
@@ -562,930 +544,525 @@
       <c r="F1" t="s">
         <v>19</v>
       </c>
-      <c r="G1" t="s">
-        <v>20</v>
-      </c>
-      <c r="H1" t="s">
-        <v>21</v>
-      </c>
-      <c r="I1" t="s">
-        <v>22</v>
-      </c>
-      <c r="J1" t="s">
-        <v>23</v>
-      </c>
-      <c r="K1" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="2">
       <c r="A2" t="s">
-        <v>25</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
       <c r="D2" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
       <c r="E2" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="F2" t="s">
-        <v>29</v>
-      </c>
-      <c r="G2" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" t="s">
-        <v>30</v>
-      </c>
-      <c r="I2" t="s">
-        <v>30</v>
-      </c>
-      <c r="J2" t="s">
-        <v>30</v>
-      </c>
-      <c r="K2" t="s">
-        <v>30</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F3" t="s">
-        <v>30</v>
-      </c>
-      <c r="G3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H3" t="s">
-        <v>30</v>
-      </c>
-      <c r="I3" t="s">
-        <v>30</v>
-      </c>
-      <c r="J3" t="s">
-        <v>30</v>
-      </c>
-      <c r="K3" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
-      </c>
-      <c r="G4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H4" t="s">
-        <v>30</v>
-      </c>
-      <c r="I4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J4" t="s">
-        <v>30</v>
-      </c>
-      <c r="K4" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
-      </c>
-      <c r="G5" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" t="s">
-        <v>30</v>
-      </c>
-      <c r="I5" t="s">
-        <v>30</v>
-      </c>
-      <c r="J5" t="s">
-        <v>30</v>
-      </c>
-      <c r="K5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
-      </c>
-      <c r="G6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H6" t="s">
-        <v>30</v>
-      </c>
-      <c r="I6" t="s">
-        <v>30</v>
-      </c>
-      <c r="J6" t="s">
-        <v>30</v>
-      </c>
-      <c r="K6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F7" t="s">
-        <v>30</v>
-      </c>
-      <c r="G7" t="s">
-        <v>30</v>
-      </c>
-      <c r="H7" t="s">
-        <v>30</v>
-      </c>
-      <c r="I7" t="s">
-        <v>30</v>
-      </c>
-      <c r="J7" t="s">
-        <v>30</v>
-      </c>
-      <c r="K7" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
-      </c>
-      <c r="G8" t="s">
-        <v>30</v>
-      </c>
-      <c r="H8" t="s">
-        <v>30</v>
-      </c>
-      <c r="I8" t="s">
-        <v>30</v>
-      </c>
-      <c r="J8" t="s">
-        <v>30</v>
-      </c>
-      <c r="K8" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F9" t="s">
-        <v>30</v>
-      </c>
-      <c r="G9" t="s">
-        <v>30</v>
-      </c>
-      <c r="H9" t="s">
-        <v>30</v>
-      </c>
-      <c r="I9" t="s">
-        <v>30</v>
-      </c>
-      <c r="J9" t="s">
-        <v>30</v>
-      </c>
-      <c r="K9" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F10" t="s">
-        <v>30</v>
-      </c>
-      <c r="G10" t="s">
-        <v>30</v>
-      </c>
-      <c r="H10" t="s">
-        <v>30</v>
-      </c>
-      <c r="I10" t="s">
-        <v>30</v>
-      </c>
-      <c r="J10" t="s">
-        <v>30</v>
-      </c>
-      <c r="K10" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F11" t="s">
-        <v>30</v>
-      </c>
-      <c r="G11" t="s">
-        <v>30</v>
-      </c>
-      <c r="H11" t="s">
-        <v>30</v>
-      </c>
-      <c r="I11" t="s">
-        <v>30</v>
-      </c>
-      <c r="J11" t="s">
-        <v>30</v>
-      </c>
-      <c r="K11" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F12" t="s">
-        <v>30</v>
-      </c>
-      <c r="G12" t="s">
-        <v>30</v>
-      </c>
-      <c r="H12" t="s">
-        <v>30</v>
-      </c>
-      <c r="I12" t="s">
-        <v>30</v>
-      </c>
-      <c r="J12" t="s">
-        <v>30</v>
-      </c>
-      <c r="K12" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B13" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C13" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D13" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E13" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F13" t="s">
-        <v>30</v>
-      </c>
-      <c r="G13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H13" t="s">
-        <v>30</v>
-      </c>
-      <c r="I13" t="s">
-        <v>30</v>
-      </c>
-      <c r="J13" t="s">
-        <v>30</v>
-      </c>
-      <c r="K13" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F14" t="s">
-        <v>30</v>
-      </c>
-      <c r="G14" t="s">
-        <v>30</v>
-      </c>
-      <c r="H14" t="s">
-        <v>30</v>
-      </c>
-      <c r="I14" t="s">
-        <v>30</v>
-      </c>
-      <c r="J14" t="s">
-        <v>30</v>
-      </c>
-      <c r="K14" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F15" t="s">
-        <v>30</v>
-      </c>
-      <c r="G15" t="s">
-        <v>30</v>
-      </c>
-      <c r="H15" t="s">
-        <v>30</v>
-      </c>
-      <c r="I15" t="s">
-        <v>30</v>
-      </c>
-      <c r="J15" t="s">
-        <v>30</v>
-      </c>
-      <c r="K15" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F16" t="s">
-        <v>30</v>
-      </c>
-      <c r="G16" t="s">
-        <v>30</v>
-      </c>
-      <c r="H16" t="s">
-        <v>30</v>
-      </c>
-      <c r="I16" t="s">
-        <v>30</v>
-      </c>
-      <c r="J16" t="s">
-        <v>30</v>
-      </c>
-      <c r="K16" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F17" t="s">
-        <v>30</v>
-      </c>
-      <c r="G17" t="s">
-        <v>30</v>
-      </c>
-      <c r="H17" t="s">
-        <v>30</v>
-      </c>
-      <c r="I17" t="s">
-        <v>30</v>
-      </c>
-      <c r="J17" t="s">
-        <v>30</v>
-      </c>
-      <c r="K17" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F18" t="s">
-        <v>30</v>
-      </c>
-      <c r="G18" t="s">
-        <v>30</v>
-      </c>
-      <c r="H18" t="s">
-        <v>30</v>
-      </c>
-      <c r="I18" t="s">
-        <v>30</v>
-      </c>
-      <c r="J18" t="s">
-        <v>30</v>
-      </c>
-      <c r="K18" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F19" t="s">
-        <v>30</v>
-      </c>
-      <c r="G19" t="s">
-        <v>30</v>
-      </c>
-      <c r="H19" t="s">
-        <v>30</v>
-      </c>
-      <c r="I19" t="s">
-        <v>30</v>
-      </c>
-      <c r="J19" t="s">
-        <v>30</v>
-      </c>
-      <c r="K19" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B20" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C20" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D20" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E20" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F20" t="s">
-        <v>30</v>
-      </c>
-      <c r="G20" t="s">
-        <v>30</v>
-      </c>
-      <c r="H20" t="s">
-        <v>30</v>
-      </c>
-      <c r="I20" t="s">
-        <v>30</v>
-      </c>
-      <c r="J20" t="s">
-        <v>30</v>
-      </c>
-      <c r="K20" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C21" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D21" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E21" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F21" t="s">
-        <v>30</v>
-      </c>
-      <c r="G21" t="s">
-        <v>30</v>
-      </c>
-      <c r="H21" t="s">
-        <v>30</v>
-      </c>
-      <c r="I21" t="s">
-        <v>30</v>
-      </c>
-      <c r="J21" t="s">
-        <v>30</v>
-      </c>
-      <c r="K21" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B22" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D22" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E22" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F22" t="s">
-        <v>30</v>
-      </c>
-      <c r="G22" t="s">
-        <v>30</v>
-      </c>
-      <c r="H22" t="s">
-        <v>30</v>
-      </c>
-      <c r="I22" t="s">
-        <v>30</v>
-      </c>
-      <c r="J22" t="s">
-        <v>30</v>
-      </c>
-      <c r="K22" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F23" t="s">
-        <v>30</v>
-      </c>
-      <c r="G23" t="s">
-        <v>30</v>
-      </c>
-      <c r="H23" t="s">
-        <v>30</v>
-      </c>
-      <c r="I23" t="s">
-        <v>30</v>
-      </c>
-      <c r="J23" t="s">
-        <v>30</v>
-      </c>
-      <c r="K23" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F24" t="s">
-        <v>30</v>
-      </c>
-      <c r="G24" t="s">
-        <v>30</v>
-      </c>
-      <c r="H24" t="s">
-        <v>30</v>
-      </c>
-      <c r="I24" t="s">
-        <v>30</v>
-      </c>
-      <c r="J24" t="s">
-        <v>30</v>
-      </c>
-      <c r="K24" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C25" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D25" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E25" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F25" t="s">
-        <v>30</v>
-      </c>
-      <c r="G25" t="s">
-        <v>30</v>
-      </c>
-      <c r="H25" t="s">
-        <v>30</v>
-      </c>
-      <c r="I25" t="s">
-        <v>30</v>
-      </c>
-      <c r="J25" t="s">
-        <v>30</v>
-      </c>
-      <c r="K25" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D26" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E26" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F26" t="s">
-        <v>30</v>
-      </c>
-      <c r="G26" t="s">
-        <v>30</v>
-      </c>
-      <c r="H26" t="s">
-        <v>30</v>
-      </c>
-      <c r="I26" t="s">
-        <v>30</v>
-      </c>
-      <c r="J26" t="s">
-        <v>30</v>
-      </c>
-      <c r="K26" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="C27" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="D27" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="E27" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F27" t="s">
-        <v>30</v>
-      </c>
-      <c r="G27" t="s">
-        <v>30</v>
-      </c>
-      <c r="H27" t="s">
-        <v>30</v>
-      </c>
-      <c r="I27" t="s">
-        <v>30</v>
-      </c>
-      <c r="J27" t="s">
-        <v>30</v>
-      </c>
-      <c r="K27" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>
@@ -1504,7 +1081,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
         <v>16</v>
@@ -1513,28 +1090,28 @@
         <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
         <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="J1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="K1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>
@@ -1553,7 +1130,7 @@
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="B1" t="s">
         <v>16</v>
@@ -1562,28 +1139,28 @@
         <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
         <v>19</v>
       </c>
       <c r="G1" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="H1" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="I1" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="J1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="K1" t="s">
-        <v>38</v>
+        <v>32</v>
       </c>
     </row>
   </sheetData>

</xml_diff>